<commit_message>
segunda versión de BBDD de InversionesHumitas 13_11
</commit_message>
<xml_diff>
--- a/BBDD.xlsx
+++ b/BBDD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\workspace\InversionesHumitas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\workspace\InversionesHumitas\RepositorioInversionesHumitas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93086CE2-BCE3-4905-82CD-386EBD834A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A78A88-69DD-49B9-A4E7-5E81D769924B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <t>DESCRIPCION</t>
   </si>
   <si>
-    <t>JEFE</t>
-  </si>
-  <si>
     <t>Responsable de uno o más almacenes</t>
   </si>
   <si>
@@ -448,7 +445,10 @@
     <t>CALZADO EXCLUSIVO PARA EL USO EN FIESTAS, EVENTOS O COMPROMISOS FORMALES</t>
   </si>
   <si>
-    <t>BASE DE DATOS DE INVERSIONES HUMITAS</t>
+    <t>BASE DE DATOS DE INVERSIONES HUMITAS - Actualizado al 13_11_2023</t>
+  </si>
+  <si>
+    <t>JEFESITO</t>
   </si>
 </sst>
 </file>
@@ -771,7 +771,7 @@
   <dimension ref="A1:J190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -788,7 +788,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="52" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
@@ -812,10 +812,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
@@ -823,10 +823,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
@@ -834,10 +834,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
@@ -845,10 +845,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
@@ -856,10 +856,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -882,7 +882,7 @@
     </row>
     <row r="10" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -896,28 +896,28 @@
     </row>
     <row r="11" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -933,13 +933,13 @@
         <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="G12" s="4">
         <v>64370246</v>
@@ -961,13 +961,13 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="4">
         <v>14328394</v>
@@ -989,13 +989,13 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="4">
         <v>69075261</v>
@@ -1017,13 +1017,13 @@
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="4">
         <v>35771553</v>
@@ -1045,13 +1045,13 @@
         <v>4</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="4">
         <v>20569226</v>
@@ -1073,13 +1073,13 @@
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" s="4">
         <v>34510069</v>
@@ -1101,13 +1101,13 @@
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18" s="4">
         <v>27595871</v>
@@ -1129,13 +1129,13 @@
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G19" s="4">
         <v>56078915</v>
@@ -1157,13 +1157,13 @@
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" s="4">
         <v>98230455</v>
@@ -1185,13 +1185,13 @@
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G21" s="4">
         <v>95373481</v>
@@ -1213,13 +1213,13 @@
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G22" s="4">
         <v>30983775</v>
@@ -1241,13 +1241,13 @@
         <v>3</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G23" s="4">
         <v>27553034</v>
@@ -1269,13 +1269,13 @@
         <v>3</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G24" s="4">
         <v>59235924</v>
@@ -1297,13 +1297,13 @@
         <v>3</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G25" s="4">
         <v>47465880</v>
@@ -1325,13 +1325,13 @@
         <v>2</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26" s="4">
         <v>88154875</v>
@@ -1366,15 +1366,15 @@
     </row>
     <row r="30" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>3</v>
@@ -1385,10 +1385,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
@@ -1396,10 +1396,10 @@
         <v>2</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
@@ -1407,10 +1407,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
@@ -1418,23 +1418,23 @@
         <v>4</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>3</v>
@@ -1445,10 +1445,10 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
@@ -1456,10 +1456,10 @@
         <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
@@ -1467,10 +1467,10 @@
         <v>3</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
@@ -1478,43 +1478,43 @@
         <v>4</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="D47" s="2">
         <v>2016</v>
@@ -1525,13 +1525,13 @@
     </row>
     <row r="48" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="D48" s="2">
         <v>2015</v>
@@ -1542,13 +1542,13 @@
     </row>
     <row r="49" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D49" s="2">
         <v>2018</v>
@@ -1559,36 +1559,36 @@
     </row>
     <row r="53" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B54" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E54" s="5" t="s">
+      <c r="F54" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="G54" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="H54" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="I54" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>11341</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F55" s="2">
         <v>2</v>
@@ -1611,7 +1611,7 @@
         <v>45184</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I55" s="2">
         <f t="shared" ref="I55:I60" si="0">SUMIF($A$64:$A$84,$B$55:$B$60,$H$64:$H$84)</f>
@@ -1629,7 +1629,7 @@
         <v>29666</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E56" s="2">
         <v>1</v>
@@ -1641,7 +1641,7 @@
         <v>45185</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I56" s="2">
         <f t="shared" si="0"/>
@@ -1659,7 +1659,7 @@
         <v>15866</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E57" s="2">
         <v>1</v>
@@ -1671,7 +1671,7 @@
         <v>45186</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I57" s="2">
         <f t="shared" si="0"/>
@@ -1689,7 +1689,7 @@
         <v>11341</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E58" s="2">
         <v>2</v>
@@ -1701,7 +1701,7 @@
         <v>45187</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I58" s="2">
         <f t="shared" si="0"/>
@@ -1719,7 +1719,7 @@
         <v>29666</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E59" s="2">
         <v>3</v>
@@ -1731,7 +1731,7 @@
         <v>45188</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I59" s="2">
         <f t="shared" si="0"/>
@@ -1749,7 +1749,7 @@
         <v>15866</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E60" s="2">
         <v>3</v>
@@ -1758,7 +1758,7 @@
         <v>45189</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I60" s="2">
         <f t="shared" si="0"/>
@@ -1767,33 +1767,33 @@
     </row>
     <row r="62" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="D63" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D63" s="5" t="s">
+      <c r="F63" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="G63" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H63" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
@@ -1813,7 +1813,7 @@
         <v>45184</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H64" s="2">
         <f t="shared" ref="H64:H84" si="1">E64*VLOOKUP(B64,$A$163:$F$183,6,0)</f>
@@ -1837,7 +1837,7 @@
         <v>45184</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" si="1"/>
@@ -1861,7 +1861,7 @@
         <v>45184</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H66" s="2">
         <f t="shared" si="1"/>
@@ -1885,7 +1885,7 @@
         <v>45184</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H67" s="2">
         <f t="shared" si="1"/>
@@ -1912,7 +1912,7 @@
         <v>45185</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" si="1"/>
@@ -1939,7 +1939,7 @@
         <v>45185</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H69" s="2">
         <f t="shared" si="1"/>
@@ -1966,7 +1966,7 @@
         <v>45185</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H70" s="2">
         <f t="shared" si="1"/>
@@ -1993,7 +1993,7 @@
         <v>45185</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H71" s="2">
         <f t="shared" si="1"/>
@@ -2020,7 +2020,7 @@
         <v>45185</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H72" s="2">
         <f t="shared" si="1"/>
@@ -2047,7 +2047,7 @@
         <v>45186</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H73" s="2">
         <f t="shared" si="1"/>
@@ -2074,7 +2074,7 @@
         <v>45187</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H74" s="2">
         <f t="shared" si="1"/>
@@ -2101,7 +2101,7 @@
         <v>45187</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H75" s="2">
         <f t="shared" si="1"/>
@@ -2128,7 +2128,7 @@
         <v>45187</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H76" s="2">
         <f t="shared" si="1"/>
@@ -2155,7 +2155,7 @@
         <v>45187</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H77" s="2">
         <f t="shared" si="1"/>
@@ -2182,7 +2182,7 @@
         <v>45187</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H78" s="2">
         <f t="shared" si="1"/>
@@ -2209,7 +2209,7 @@
         <v>45187</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H79" s="2">
         <f t="shared" si="1"/>
@@ -2236,7 +2236,7 @@
         <v>45187</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H80" s="2">
         <f t="shared" si="1"/>
@@ -2263,7 +2263,7 @@
         <v>45187</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H81" s="2">
         <f t="shared" si="1"/>
@@ -2290,7 +2290,7 @@
         <v>45188</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H82" s="2">
         <f t="shared" si="1"/>
@@ -2317,7 +2317,7 @@
         <v>45188</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H83" s="2">
         <f t="shared" si="1"/>
@@ -2341,7 +2341,7 @@
         <v>45189</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H84" s="2">
         <f t="shared" si="1"/>
@@ -2368,21 +2368,21 @@
     </row>
     <row r="89" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="D90" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
@@ -2390,10 +2390,10 @@
         <v>1</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="D91" s="2">
         <v>5000</v>
@@ -2404,10 +2404,10 @@
         <v>2</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="D92" s="2">
         <v>2500</v>
@@ -2418,10 +2418,10 @@
         <v>3</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D93" s="2">
         <v>1500</v>
@@ -2429,18 +2429,18 @@
     </row>
     <row r="97" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -3107,30 +3107,30 @@
     <row r="160" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="162" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="163" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B163" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D163" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C163" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D163" s="5" t="s">
+      <c r="E163" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E163" s="5" t="s">
+      <c r="F163" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F163" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="G163" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="164" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
@@ -3141,13 +3141,13 @@
         <v>2</v>
       </c>
       <c r="C164" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D164" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D164" s="3" t="s">
+      <c r="E164" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="F164" s="3">
         <v>0.15</v>
@@ -3167,13 +3167,13 @@
         <v>2</v>
       </c>
       <c r="C165" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D165" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D165" s="3" t="s">
+      <c r="E165" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="F165" s="3">
         <v>0.17</v>
@@ -3193,13 +3193,13 @@
         <v>3</v>
       </c>
       <c r="C166" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D166" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D166" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="E166" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F166" s="3">
         <v>0.15</v>
@@ -3219,13 +3219,13 @@
         <v>1</v>
       </c>
       <c r="C167" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D167" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D167" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="E167" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F167" s="3">
         <v>0.15</v>
@@ -3245,13 +3245,13 @@
         <v>2</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D168" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E168" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="E168" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="F168" s="3">
         <v>0.15</v>
@@ -3271,13 +3271,13 @@
         <v>2</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F169" s="3">
         <v>0.15</v>
@@ -3297,13 +3297,13 @@
         <v>3</v>
       </c>
       <c r="C170" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D170" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D170" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="E170" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F170" s="3">
         <v>0.17</v>
@@ -3323,13 +3323,13 @@
         <v>3</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F171" s="3">
         <v>0.15</v>
@@ -3349,13 +3349,13 @@
         <v>1</v>
       </c>
       <c r="C172" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D172" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D172" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="E172" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F172" s="3">
         <v>0.17</v>
@@ -3375,13 +3375,13 @@
         <v>1</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F173" s="3">
         <v>0.15</v>
@@ -3401,13 +3401,13 @@
         <v>3</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F174" s="3">
         <v>0.17</v>
@@ -3427,13 +3427,13 @@
         <v>2</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F175" s="3">
         <v>0.19</v>
@@ -3453,13 +3453,13 @@
         <v>2</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D176" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E176" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="E176" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="F176" s="3">
         <v>0.17</v>
@@ -3479,13 +3479,13 @@
         <v>2</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D177" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E177" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="E177" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="F177" s="3">
         <v>0.15</v>
@@ -3505,13 +3505,13 @@
         <v>2</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D178" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E178" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="E178" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="F178" s="3">
         <v>0.17</v>
@@ -3531,13 +3531,13 @@
         <v>3</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F179" s="3">
         <v>0.15</v>
@@ -3557,13 +3557,13 @@
         <v>1</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F180" s="3">
         <v>0.17</v>
@@ -3583,13 +3583,13 @@
         <v>2</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F181" s="3">
         <v>0.17</v>
@@ -3609,13 +3609,13 @@
         <v>2</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F182" s="3">
         <v>0.15</v>
@@ -3635,13 +3635,13 @@
         <v>1</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F183" s="3">
         <v>0.15</v>
@@ -3655,15 +3655,15 @@
     </row>
     <row r="186" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="187" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C187" s="5" t="s">
         <v>3</v>
@@ -3674,10 +3674,10 @@
         <v>1</v>
       </c>
       <c r="B188" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C188" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C188" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="189" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
@@ -3685,10 +3685,10 @@
         <v>2</v>
       </c>
       <c r="B189" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C189" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="190" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
@@ -3696,10 +3696,10 @@
         <v>3</v>
       </c>
       <c r="B190" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C190" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>